<commit_message>
fixbug kal001 : #105606
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KAL001-アラームリスト(個人別).xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KAL001-アラームリスト(個人別).xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CDEE08-EA09-4486-948A-88B8ACBFEC12}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="0" windowWidth="20490" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13845" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="帳票テンプレート" sheetId="2" r:id="rId1"/>
@@ -105,7 +104,7 @@
     <definedName name="PG田中" localSheetId="0">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">帳票テンプレート!$A$2:$H$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">帳票テンプレート!$2:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">帳票テンプレート!$1:$2</definedName>
     <definedName name="PrintDaicho" localSheetId="0">[7]!PrintDaicho</definedName>
     <definedName name="PrintDaicho">[7]!PrintDaicho</definedName>
     <definedName name="QuitDaicho" localSheetId="0">[7]!QuitDaicho</definedName>
@@ -230,7 +229,8 @@
     <definedName name="飛行機" localSheetId="0">#REF!</definedName>
     <definedName name="飛行機">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -371,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -394,11 +394,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -413,9 +422,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -43704,7 +43716,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -43779,23 +43791,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -43831,23 +43826,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -44023,11 +44001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -44041,7 +44019,17 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -44067,7 +44055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="36" customHeight="1">
+    <row r="3" spans="1:11" ht="36" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -44093,17 +44081,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1"/>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1"/>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1"/>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1"/>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1"/>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1"/>
-    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1"/>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1"/>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1"/>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1"/>
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L日通システム株式会社

</xml_diff>